<commit_message>
rodando modelo com resultado plausível
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="170">
   <si>
     <t>Variavel</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>Replicação</t>
+  </si>
+  <si>
+    <t>Incerto</t>
   </si>
 </sst>
 </file>
@@ -1000,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1014,7 @@
     <col min="3" max="3" width="12.28515625" style="2"/>
     <col min="4" max="4" width="13.42578125" style="2"/>
     <col min="5" max="5" width="17.85546875" style="1"/>
-    <col min="6" max="6" width="4.7109375" style="2"/>
+    <col min="6" max="6" width="6.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" style="1"/>
     <col min="8" max="8" width="10.7109375" style="1"/>
     <col min="9" max="9" width="7" style="1"/>
@@ -1559,17 +1562,17 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>50000</v>
+        <v>45000</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>50000</v>
+        <v>55000</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G13">
         <f>J13/10</f>
@@ -1580,7 +1583,7 @@
         <v>500000</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>17</v>
+        <v>169</v>
       </c>
       <c r="J13" s="5">
         <v>50000</v>
@@ -1592,7 +1595,7 @@
       <c r="M13"/>
       <c r="N13" s="1" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ativando o setor de patentes e PeD - checks passando
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao.xlsx
@@ -1003,8 +1003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1023,8 @@
     <col min="11" max="11" width="8" style="1"/>
     <col min="12" max="12" width="10.140625" style="1"/>
     <col min="13" max="13" width="9.7109375" style="1"/>
-    <col min="14" max="1023" width="7" style="1"/>
+    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
+    <col min="15" max="1023" width="7" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2677,11 +2679,11 @@
       </c>
       <c r="C38" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>20</v>
@@ -2699,7 +2701,7 @@
         <v>17</v>
       </c>
       <c r="J38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="1">
         <v>0</v>
@@ -3296,28 +3298,28 @@
       <c r="B55"/>
       <c r="C55" s="2">
         <f t="shared" si="3"/>
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="D55" s="2">
         <f t="shared" si="4"/>
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="F55" s="2">
         <v>0.5</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="6"/>
-        <v>250000</v>
+        <v>500000</v>
       </c>
       <c r="H55" s="1">
         <f t="shared" si="7"/>
-        <v>4000000</v>
+        <v>8000000</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J55" s="1">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="K55" s="1">
         <v>1000000</v>
@@ -3331,11 +3333,11 @@
         <v>130</v>
       </c>
       <c r="C56" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C56:C62" si="8">IF(I56="Incerto",MAX(G56,J56-(ABS(F56*J56))),J56)</f>
         <v>0.5</v>
       </c>
       <c r="D56" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D56:D62" si="9">IF(I56="Incerto",MIN(H56,J56+(ABS(F56*J56))),J56)</f>
         <v>0.5</v>
       </c>
       <c r="F56" s="2">
@@ -3377,6 +3379,9 @@
         <f>C57</f>
         <v>0.5</v>
       </c>
+      <c r="K57" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -3396,6 +3401,10 @@
         <f>C58</f>
         <v>0.4</v>
       </c>
+      <c r="K58" s="1">
+        <f>D58</f>
+        <v>0.4</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -3415,6 +3424,10 @@
         <f>C59</f>
         <v>2500</v>
       </c>
+      <c r="K59" s="1">
+        <f>D59</f>
+        <v>2500</v>
+      </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
@@ -3434,16 +3447,29 @@
         <f>C60</f>
         <v>1831</v>
       </c>
+      <c r="K60" s="1">
+        <f>D60</f>
+        <v>1831</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B61"/>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
       <c r="I61" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J61" s="1">
+        <v>1</v>
+      </c>
+      <c r="K61" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3452,10 +3478,19 @@
         <v>136</v>
       </c>
       <c r="B62"/>
+      <c r="C62" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.3</v>
+      </c>
       <c r="I62" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J62" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="K62" s="1">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>